<commit_message>
Added catches for unexpected/malformed data
</commit_message>
<xml_diff>
--- a/tools/IJE_File_Layouts_Input_Mapping_WA_Version_2021.xlsx
+++ b/tools/IJE_File_Layouts_Input_Mapping_WA_Version_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rscalfani/Documents/code/NVSS/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6AB9E0-D2C4-6C46-9F22-06DEC6C64270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935F0586-CB10-2C4E-B5AA-8B5242FC0165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20500" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality_Trim_mappings" sheetId="2" r:id="rId1"/>
@@ -2968,13 +2968,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="45" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3322,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD74E696-0F05-DF43-9EB9-28DAB6A6F493}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3331,32 +3331,32 @@
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="75" t="s">
         <v>626</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="75" t="s">
         <v>627</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="75" t="s">
         <v>726</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="75" t="s">
         <v>700</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="75" t="s">
         <v>657</v>
       </c>
     </row>
@@ -9996,7 +9996,7 @@
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="D68" s="75" t="s">
+      <c r="D68" s="76" t="s">
         <v>168</v>
       </c>
       <c r="E68" s="8" t="s">
@@ -10029,7 +10029,7 @@
       <c r="C69" s="6">
         <v>3</v>
       </c>
-      <c r="D69" s="75"/>
+      <c r="D69" s="76"/>
       <c r="E69" s="8" t="s">
         <v>171</v>
       </c>
@@ -10060,7 +10060,7 @@
       <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="D70" s="75"/>
+      <c r="D70" s="76"/>
       <c r="E70" s="8" t="s">
         <v>173</v>
       </c>
@@ -10091,7 +10091,7 @@
       <c r="C71" s="6">
         <v>3</v>
       </c>
-      <c r="D71" s="75"/>
+      <c r="D71" s="76"/>
       <c r="E71" s="8" t="s">
         <v>174</v>
       </c>
@@ -10122,7 +10122,7 @@
       <c r="C72" s="6">
         <v>3</v>
       </c>
-      <c r="D72" s="75"/>
+      <c r="D72" s="76"/>
       <c r="E72" s="8" t="s">
         <v>175</v>
       </c>
@@ -10153,7 +10153,7 @@
       <c r="C73" s="6">
         <v>3</v>
       </c>
-      <c r="D73" s="75"/>
+      <c r="D73" s="76"/>
       <c r="E73" s="8" t="s">
         <v>176</v>
       </c>
@@ -10184,7 +10184,7 @@
       <c r="C74" s="6">
         <v>3</v>
       </c>
-      <c r="D74" s="75"/>
+      <c r="D74" s="76"/>
       <c r="E74" s="8" t="s">
         <v>177</v>
       </c>
@@ -10215,7 +10215,7 @@
       <c r="C75" s="6">
         <v>3</v>
       </c>
-      <c r="D75" s="75"/>
+      <c r="D75" s="76"/>
       <c r="E75" s="8" t="s">
         <v>178</v>
       </c>
@@ -10246,7 +10246,7 @@
       <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="D76" s="75"/>
+      <c r="D76" s="76"/>
       <c r="E76" s="8" t="s">
         <v>179</v>
       </c>
@@ -10277,7 +10277,7 @@
       <c r="C77" s="6">
         <v>3</v>
       </c>
-      <c r="D77" s="75"/>
+      <c r="D77" s="76"/>
       <c r="E77" s="8" t="s">
         <v>180</v>
       </c>
@@ -10308,7 +10308,7 @@
       <c r="C78" s="6">
         <v>3</v>
       </c>
-      <c r="D78" s="75"/>
+      <c r="D78" s="76"/>
       <c r="E78" s="8" t="s">
         <v>181</v>
       </c>
@@ -10339,7 +10339,7 @@
       <c r="C79" s="6">
         <v>3</v>
       </c>
-      <c r="D79" s="75"/>
+      <c r="D79" s="76"/>
       <c r="E79" s="8" t="s">
         <v>182</v>
       </c>
@@ -10370,7 +10370,7 @@
       <c r="C80" s="6">
         <v>3</v>
       </c>
-      <c r="D80" s="75"/>
+      <c r="D80" s="76"/>
       <c r="E80" s="8" t="s">
         <v>183</v>
       </c>
@@ -10401,7 +10401,7 @@
       <c r="C81" s="6">
         <v>3</v>
       </c>
-      <c r="D81" s="75"/>
+      <c r="D81" s="76"/>
       <c r="E81" s="8" t="s">
         <v>184</v>
       </c>
@@ -10432,7 +10432,7 @@
       <c r="C82" s="6">
         <v>3</v>
       </c>
-      <c r="D82" s="75"/>
+      <c r="D82" s="76"/>
       <c r="E82" s="8" t="s">
         <v>185</v>
       </c>
@@ -10463,7 +10463,7 @@
       <c r="C83" s="6">
         <v>3</v>
       </c>
-      <c r="D83" s="75"/>
+      <c r="D83" s="76"/>
       <c r="E83" s="8" t="s">
         <v>186</v>
       </c>
@@ -11043,7 +11043,7 @@
       <c r="F101" s="24" t="s">
         <v>685</v>
       </c>
-      <c r="G101" s="76" t="s">
+      <c r="G101" s="77" t="s">
         <v>227</v>
       </c>
       <c r="H101" s="22" t="s">
@@ -11074,7 +11074,7 @@
       <c r="F102" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="G102" s="76"/>
+      <c r="G102" s="77"/>
       <c r="H102" s="36"/>
       <c r="I102" s="7" t="s">
         <v>706</v>
@@ -11106,7 +11106,7 @@
       <c r="F103" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="G103" s="76"/>
+      <c r="G103" s="77"/>
       <c r="H103" s="36"/>
       <c r="I103" s="7" t="s">
         <v>706</v>
@@ -11137,7 +11137,7 @@
       <c r="F104" s="24" t="s">
         <v>686</v>
       </c>
-      <c r="G104" s="76"/>
+      <c r="G104" s="77"/>
       <c r="H104" s="22" t="s">
         <v>727</v>
       </c>
@@ -11168,7 +11168,7 @@
       <c r="F105" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="G105" s="76"/>
+      <c r="G105" s="77"/>
       <c r="H105" s="22" t="s">
         <v>727</v>
       </c>
@@ -11197,7 +11197,7 @@
       <c r="F106" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="G106" s="76"/>
+      <c r="G106" s="77"/>
       <c r="H106" s="36"/>
       <c r="I106" s="36" t="s">
         <v>706</v>
@@ -11228,7 +11228,7 @@
       <c r="F107" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="G107" s="76"/>
+      <c r="G107" s="77"/>
       <c r="H107" s="36"/>
       <c r="I107" s="36" t="s">
         <v>706</v>
@@ -11259,7 +11259,7 @@
       <c r="F108" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="G108" s="76"/>
+      <c r="G108" s="77"/>
       <c r="H108" s="36"/>
       <c r="I108" s="36" t="s">
         <v>706</v>
@@ -11290,7 +11290,7 @@
       <c r="F109" s="33" t="s">
         <v>707</v>
       </c>
-      <c r="G109" s="76"/>
+      <c r="G109" s="77"/>
       <c r="H109" s="22" t="s">
         <v>727</v>
       </c>
@@ -11321,7 +11321,7 @@
       <c r="F110" s="24" t="s">
         <v>689</v>
       </c>
-      <c r="G110" s="76"/>
+      <c r="G110" s="77"/>
       <c r="H110" s="22" t="s">
         <v>727</v>
       </c>
@@ -11350,7 +11350,7 @@
       <c r="F111" s="24" t="s">
         <v>690</v>
       </c>
-      <c r="G111" s="76"/>
+      <c r="G111" s="77"/>
       <c r="H111" s="22" t="s">
         <v>727</v>
       </c>
@@ -11379,7 +11379,7 @@
       <c r="F112" s="24" t="s">
         <v>691</v>
       </c>
-      <c r="G112" s="76"/>
+      <c r="G112" s="77"/>
       <c r="H112" s="22" t="s">
         <v>727</v>
       </c>
@@ -11408,7 +11408,7 @@
       <c r="F113" s="24" t="s">
         <v>692</v>
       </c>
-      <c r="G113" s="76"/>
+      <c r="G113" s="77"/>
       <c r="H113" s="22" t="s">
         <v>727</v>
       </c>
@@ -11437,7 +11437,7 @@
       <c r="F114" s="70" t="s">
         <v>630</v>
       </c>
-      <c r="G114" s="76"/>
+      <c r="G114" s="77"/>
       <c r="H114" s="36"/>
       <c r="I114" s="36" t="s">
         <v>706</v>
@@ -11466,7 +11466,7 @@
       <c r="F115" s="24" t="s">
         <v>693</v>
       </c>
-      <c r="G115" s="76"/>
+      <c r="G115" s="77"/>
       <c r="H115" s="22" t="s">
         <v>727</v>
       </c>
@@ -11495,7 +11495,7 @@
       <c r="F116" s="24" t="s">
         <v>694</v>
       </c>
-      <c r="G116" s="76"/>
+      <c r="G116" s="77"/>
       <c r="H116" s="22" t="s">
         <v>727</v>
       </c>
@@ -11524,7 +11524,7 @@
       <c r="F117" s="24" t="s">
         <v>630</v>
       </c>
-      <c r="G117" s="76"/>
+      <c r="G117" s="77"/>
       <c r="H117" s="22"/>
       <c r="I117" s="36">
         <v>2022</v>
@@ -11555,7 +11555,7 @@
       <c r="F118" s="24" t="s">
         <v>695</v>
       </c>
-      <c r="G118" s="76"/>
+      <c r="G118" s="77"/>
       <c r="H118" s="22" t="s">
         <v>727</v>
       </c>
@@ -11584,7 +11584,7 @@
       <c r="F119" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="G119" s="76"/>
+      <c r="G119" s="77"/>
       <c r="H119" s="22" t="s">
         <v>727</v>
       </c>
@@ -11613,7 +11613,7 @@
       <c r="F120" s="24" t="s">
         <v>696</v>
       </c>
-      <c r="G120" s="76"/>
+      <c r="G120" s="77"/>
       <c r="H120" s="22" t="s">
         <v>727</v>
       </c>
@@ -11642,7 +11642,7 @@
       <c r="F121" s="70" t="s">
         <v>630</v>
       </c>
-      <c r="G121" s="76"/>
+      <c r="G121" s="77"/>
       <c r="H121" s="36"/>
       <c r="I121" s="36" t="s">
         <v>706</v>
@@ -11672,7 +11672,7 @@
       <c r="F122" s="70" t="s">
         <v>630</v>
       </c>
-      <c r="G122" s="76"/>
+      <c r="G122" s="77"/>
       <c r="H122" s="36"/>
       <c r="I122" s="36" t="s">
         <v>706</v>
@@ -15804,10 +15804,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d8a0f530da2fdbe2e55626e9ad23fb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d278552e3c3a0a08e9db34919b560943" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -16029,7 +16040,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -16038,18 +16049,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -16057,7 +16068,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0A455F-891F-4D48-ABA8-1B564ACEA7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16077,21 +16088,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>